<commit_message>
add more website and Compact list.json
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Git\Anisdora-ChromeExt\awesome-websites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34ADFBCF-1B84-4694-81BF-6ED12850C48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED62F87-686A-4AD0-B2C0-E39ED8A1B80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="475">
   <si>
     <t>tags</t>
   </si>
@@ -1877,6 +1877,1133 @@
   </si>
   <si>
     <t>Pocket Monster pedia.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://makezine.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Makezine</t>
+  </si>
+  <si>
+    <t>Make: DIY Projects and Ideas for Makers.Celebrates your right to tweak, hack, and bend any technology to your will.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIY,Geek</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.psychologytoday.com/intl</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Psychology Today</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Psychology</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>View the latest from the world of psychology: from behavioral research to practical guidance on relationships, mental health and addiction. Find help from our directory of therapists, psychologists and counselors.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/theschooloflifetv</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The School of Life Channel of Youtube</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Life,Psychology,Philosophy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The School of Life is a collective of psychologists, philosophers and writers devoted to helping people lead calmer and more resilient lives. We share ideas on how to understand ourselves better, improve our relationships, take stock of our careers and deepen our social connections - as w</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.chalkstreet.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChalkStreet is an online learning marketplace which provides high quality courses from the best teachers. ChalkStreet aspires to make learning a habit.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChalkStreet</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn Something New Every Day. Each morning, wake up to a new 5-minute lesson delivered to your email inbox. Choose from 300+ topics.
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://gohighbrow.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HIGHBROW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning,Expand knowledge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://instanerd.me/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instanerd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn some interesting knowledge.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.flowkey.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flowkey</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning,Piano</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning piano Online</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bigthink.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Think,Article,Pioneer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Big think.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Big Think</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.pluralsight.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pluralsight</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code,Learning</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pluralsight is the technology workforce development company that helps teams know more and work better together with stronger skills, improved processes and informed leaders.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ideas.ted.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDEAS.TED.COM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Explore ideas worth spreading</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.wikiwand.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wikiwand</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The world's leading Wikipedia reader</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wikipedia,Reader,Software</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.uopeople.edu/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uopeople</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self-learning</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>University of the People is a tuition-free, American accredited, online college. Higher-education is now more accessible than ever.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.opensesame.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transform your workforce with thousands of eLearning courses from the world’s top publishers. Our engaging online courses work perfectly in your LMS.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenSesame</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.creativelive.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreativeLive</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Online classes in photography, art, design, craft &amp;amp; DIY, marketing, business, and entrepreneurship.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.thinkful.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thinkful is a career accelerator that gets graduates careers in tech. Learn data science or learn to code with a bootcamp-style curriculum and 1-on-1 mentorship.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thinkful</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://zidbits.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zidbits</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn interesting things and explore the mysteries of life.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Digital Photography School</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Photography,Course,Tips</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://digital-photography-school.com/tips/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Photography skills and tutorials.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.scientificamerican.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scientific American</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Science</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scientific American is the essential guide to the most awe-inspiring advances in science and technology, explaining how they change our understanding of the world and shape our lives.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.p2pu.org/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2PU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grassroots community supporting equitable, empowering peer learning in public spaces worldwide.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Education,Self-learning</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ocw.mit.edu/index.htm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIT OpenCourseWare</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self-learning,Online Course</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIT OpenCourseWare is a web-based publication of virtually all MIT course content. OCW is open and available to the world and is a permanent MIT activity.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.edx.org/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Access 2000 free online courses from 140 leading institutions worldwide. Gain new skills and earn a certificate of completion.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>edX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.mentalfloss.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mental Floss</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magazine,Fun,Trivia,Quizzes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test your knowledge with amazing and interesting facts, trivia, quizzes, and brain teaser games on MentalFloss.com.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.datacamp.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DataCamp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>One-on-one,Code,Data Science,Self-learning</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning,Data Science,R,Python</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn Data Science from the comfort of your browser, at your own pace with DataCamp's video tutorials &amp; coding challenges on R, Python, Statistics &amp; more.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CoffeeStrap </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.coffeestrap.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning,Language</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn how to speak fluently by talking with people like you.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://aeon.co/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aeon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Think,Idea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://nautil.us/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nautil</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nautilus is a different kind of science magazine. We deliver big-picture science by reporting on a single monthly topic from multiple perspectives. Read a new chapter in the story every Thursday.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Science,Magazine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aeon is a magazine of ideas and culture. We publish in-depth essays, incisive articles, and a mix of original and curated videos — free to all.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Think,Culture,Idea,Science,Magazine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://pdfbear.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PDFBEAR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pdf,Tools</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>100% Free online platform that converts, edits and transforms PDF files. We make sure that you have the right conversion tool at your disposal.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.memrise.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memrise</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Language,Learning</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn a language with thousands of video clips of real native speakers, fun and effective games to practice your skills.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://curious.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Curious</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A daily learning workout with daily curios, challenging puzzles, and 25,000+ video lessons recommended just for you.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning,Cooking,Photography,Excel,Math</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://nowiknow.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NowIKnow</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn new things by email every day.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning,By-Email</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.gushiwen.cn/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>古诗文网</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>古诗,古词,古文</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>专注于古诗文服务，致力于让古诗文爱好者更便捷地发表及获取古诗文相关资料。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://spray.training/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>spray.training</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spray,Training,Game</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FPS game gun pressing training</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.zwcsm.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天中午吃什么？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择困难症,吃饭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天中午吃什么选择</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.nihaowua.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你好污啊</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>撩汉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>撩妹,套路,金句</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>撩汉/撩妹金句</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://fakeupdate.net/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FakeUpdate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OS,Software,Update,Fake</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Windows or MacOs or other software with fake update screens.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://clash.me/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Clash allows you to type messages linked from popular music, movies, TV, YouTube and countless other sources. Or assign your favorite clips to a button to play whenever the time is right. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clash</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Audio experiment,Message</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://happyhappyhardcore.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>happy happy hardcore</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>it never hits the corner</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://itneverhitsthecorner.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classic DVD playback.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://neave.tv/</t>
+  </si>
+  <si>
+    <t>Neave.TV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Channel-hop through a collection of weird and bewildering videos.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rainymood.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rainy Mood</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rain Sounds.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://virtocean.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Virtocean</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sound,Ocean</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sound,Rainy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ocean sounds.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://purrli.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Purrli</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Purrli recreates the sound and the presence of a cat.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cat,Purr</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.meteorshowers.org/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meteor shower</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meteor shower,3D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D visualization of NASA meteor shower data.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.yini.org/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>秘密花园</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Literature,X</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://nathanfriend.io/inspiral-web/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inspiral Web</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The web version of the Inspiral app.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flowering curve,Inspiral</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://nipponcolors.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NIPPON COLORS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colors,Nippon colors</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Traditional Colors of Nippon (Japan).</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://zhongguose.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国色</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国,颜色</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>提供各种中国的传统颜色的名称，CMYK值，RGB值，16进制表示。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.prettyscale.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Am I pretty or ugly?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Face beauty analysis test.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test,Face</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://dccxi.com/trust/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>信任的进化</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>信任,人性,游戏</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个关于我们为什么和如何相互信任的游戏。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://taiko.bui.pm/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>太鼓ウェブ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">パソコンとスマホのブラウザ向けの太鼓の達人シミュレータ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="3"/>
+      </rPr>
+      <t>🥁</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> Taiko no Tatsujin rhythm game simulator for desktop and mobile browsers</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Game,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>太鼓の達人</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.sketchswap.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sketch Swap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Submit your own paintings in exchange for others' paintings</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sketch,Swap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://lines.frvr.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Play Lines FRVR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beautiful, easy to learn dots and lines puzzle game</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.getbadnews.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bad News</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drop all pretense of ethics and choose the path that builds your persona as an unscrupulous media magnate. Your task is to get as many followers as you can while slowly building up fake credibility as a news site.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.foddy.net/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foddy.net</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Games by Bennett Foddy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game,QWOP,GIRP,CLOP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://aidn.jp/mikutap/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mikutap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game,Mikutap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>クリック/タッチすることで、モーショングラフィックスと共に音を奏でるインタラクティブコンテンツの初音ミク版。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ncase.me/door/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>it's a(door)able</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game,X</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A one-minute minigame.Finally, there is an "I" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="3"/>
+      </rPr>
+      <t>♥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> U"</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://tholman.com/texter/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Texter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A creative tool that allows you to draw with words.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Draw,Words</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://magickeyboard.io/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magic Keyboard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce pressure.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game,Relax</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://findingho.me/</t>
+  </si>
+  <si>
+    <t>Finding Home is an interactive experiment. Move your mouse to interact.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>// Finding Home \\</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game,Relax,Music</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.staggeringbeauty.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Staggering Beauty</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://dos.zczc.cz/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在线 DOS 游戏</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在浏览器中在线游玩 DOS 游戏与 DOS 游戏下载！</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="3"/>
+      </rPr>
+      <t>🎮</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.famicn.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>体验那些历史上上由中国大陆及港澳台开发者开发的，以家用游戏机和掌上游戏机为平台的电子游戏。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game,Museum,History</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>中文家用游戏博物馆</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.oldmanemu.net/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>老男人游戏网</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game,PSP,PSV,PS3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>仓储式主机资源站。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://neave.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neave Interactive</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apps from Neave Interactive, including Zoom Earth, Webcam Toy, Strobe Illusion, Bouncy Balls and more.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BestGames.Com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.bestgames.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interactive Games,Collection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>We offer you the best online games chosen by the editors of bestgames.com. Including action, multiplayer, shooting, Racing, sport, io games and more at bestgames.com.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.igcd.net/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IGCD.net</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Internet Game Cars Database.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://info.cern.ch/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://info.cern.ch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The first website in the world.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://worlds-highest-website.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The world's highest website</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Website,Most X</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The World’s Highest Website</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>World's Longest Website</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.worldslongestwebsite.com/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>worldslongestwebsite</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1884,7 +3011,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1956,6 +3083,19 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI Symbol"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1978,7 +3118,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2019,6 +3159,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2301,17 +3444,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.77734375" style="7" customWidth="1"/>
     <col min="2" max="2" width="30.5546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="62.33203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="46" style="11" customWidth="1"/>
     <col min="4" max="4" width="83.77734375" style="7" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -3112,6 +4255,972 @@
       </c>
       <c r="D57" s="7" t="s">
         <v>206</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C102" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="C103" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="C105" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>401</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="C111" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C112" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="C113" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="C114" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="D114" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="C115" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="D115" s="7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="C116" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="D116" s="7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="C117" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="C118" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="C119" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="C120" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="C122" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="C124" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="D124" s="7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="C126" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -3144,8 +5253,76 @@
     <hyperlink ref="A56" r:id="rId25" xr:uid="{FCB68D9A-0E22-4D70-A3D9-9B410654B54A}"/>
     <hyperlink ref="A57" r:id="rId26" xr:uid="{C7E633B7-B25B-4E15-A14C-1D71708E4993}"/>
     <hyperlink ref="A22" r:id="rId27" xr:uid="{EE1F8B35-E628-4978-9025-C45FC3AB8199}"/>
+    <hyperlink ref="A58" r:id="rId28" xr:uid="{717D71AF-3524-4662-A137-0F654F498C0E}"/>
+    <hyperlink ref="A59" r:id="rId29" xr:uid="{10EF2740-A9C2-4A80-BE49-A9593419D2F5}"/>
+    <hyperlink ref="A60" r:id="rId30" xr:uid="{CD575FAE-0B7E-45C2-8112-BE28A4C0E9D3}"/>
+    <hyperlink ref="A61" r:id="rId31" xr:uid="{378D61D4-3C51-49BB-AA88-2E8E27AA635A}"/>
+    <hyperlink ref="A62" r:id="rId32" xr:uid="{BDB77D1F-D2F2-4C57-BBC6-F499D0E9BA11}"/>
+    <hyperlink ref="A63" r:id="rId33" xr:uid="{A1197ACC-07AF-40D0-B1AE-97C0434C9EAC}"/>
+    <hyperlink ref="A64" r:id="rId34" xr:uid="{805AB297-97BC-4204-82CD-B7AEF3000DAD}"/>
+    <hyperlink ref="A65" r:id="rId35" xr:uid="{5EFB8C55-EDEA-4B42-8DD8-F11C32F62CF4}"/>
+    <hyperlink ref="A66" r:id="rId36" xr:uid="{862A0459-9D7D-42A1-9B61-51DD3D17F717}"/>
+    <hyperlink ref="A67" r:id="rId37" xr:uid="{FCE8498F-9766-45F2-AE6A-2913209C732D}"/>
+    <hyperlink ref="A68" r:id="rId38" xr:uid="{AFEA3B9C-008F-4293-9261-B31A03B13E29}"/>
+    <hyperlink ref="A69" r:id="rId39" xr:uid="{66145CF0-5F2B-4F8A-9577-8CF389E43F42}"/>
+    <hyperlink ref="A70" r:id="rId40" xr:uid="{031C1C0C-ABD5-4C37-87C4-6F280CA76D0C}"/>
+    <hyperlink ref="A71" r:id="rId41" xr:uid="{BC9652C1-C0CB-4C92-BE5B-57E8382358B4}"/>
+    <hyperlink ref="A72" r:id="rId42" xr:uid="{BE6348A5-ECB2-4D63-903A-C7F7FCCAF640}"/>
+    <hyperlink ref="A73" r:id="rId43" xr:uid="{30431339-2B9A-422C-A034-5D3FEAC310D6}"/>
+    <hyperlink ref="A74" r:id="rId44" xr:uid="{DF5E0DD3-CF9D-4EB7-8775-648F660320B5}"/>
+    <hyperlink ref="A75" r:id="rId45" xr:uid="{67B28AE1-3028-43A9-8B6C-CCA183B1D58E}"/>
+    <hyperlink ref="A76" r:id="rId46" xr:uid="{C6B0731E-9D94-4AA4-AE9B-12D758340C36}"/>
+    <hyperlink ref="A77" r:id="rId47" xr:uid="{0B1040B2-FE42-4E35-BD03-5C7335C2B6FD}"/>
+    <hyperlink ref="A78" r:id="rId48" xr:uid="{7373B62A-8800-42FF-BCDB-06D63861FB4E}"/>
+    <hyperlink ref="A79" r:id="rId49" xr:uid="{B5DC3528-C7AA-4A76-BC13-C84525B94649}"/>
+    <hyperlink ref="A80" r:id="rId50" xr:uid="{4C452E16-C551-4195-B3D8-0CF008F125DE}"/>
+    <hyperlink ref="A81" r:id="rId51" xr:uid="{7D35EC14-1793-4433-A684-3A159CC97815}"/>
+    <hyperlink ref="A82" r:id="rId52" xr:uid="{7E38DBB3-5F54-4105-BB37-5E54FEE2D473}"/>
+    <hyperlink ref="A83" r:id="rId53" xr:uid="{799D3D31-D377-4525-9F77-817606690086}"/>
+    <hyperlink ref="A84" r:id="rId54" xr:uid="{E7D6AC81-B8B1-4688-8CFA-2166D99BEE80}"/>
+    <hyperlink ref="A85" r:id="rId55" xr:uid="{F3FCF22D-25E3-4FFF-9FF4-E3C9B08556CC}"/>
+    <hyperlink ref="A86" r:id="rId56" xr:uid="{BA544344-5AD8-4B69-AE82-C5E63FDDA011}"/>
+    <hyperlink ref="A87" r:id="rId57" xr:uid="{8CF6CC04-68B0-47E4-A652-9C85C16429E7}"/>
+    <hyperlink ref="A88" r:id="rId58" xr:uid="{04D0D91A-28BF-40F3-80E3-01973CB25B03}"/>
+    <hyperlink ref="A89" r:id="rId59" xr:uid="{D06BC39E-CC8D-4455-80CC-DCA6B787100D}"/>
+    <hyperlink ref="A90" r:id="rId60" xr:uid="{C12F47E3-84A7-4942-8D62-D7027FA96CAB}"/>
+    <hyperlink ref="A91" r:id="rId61" xr:uid="{5FAE64E6-A2E1-4693-BDA5-1D4D51CABCA8}"/>
+    <hyperlink ref="A92" r:id="rId62" xr:uid="{E298FF14-69A9-4AD7-860A-CDB7DC25AB28}"/>
+    <hyperlink ref="A93" r:id="rId63" xr:uid="{E8527097-D9DD-4174-A328-49330642E718}"/>
+    <hyperlink ref="A94" r:id="rId64" xr:uid="{DF5F4A94-0350-494E-85CA-EC91FB2C430D}"/>
+    <hyperlink ref="A95" r:id="rId65" xr:uid="{35DD272C-0C74-4EFA-9F32-8946FEF00E10}"/>
+    <hyperlink ref="A97" r:id="rId66" xr:uid="{76EF1813-3F14-4D6F-9032-BA29EFC6FBCD}"/>
+    <hyperlink ref="A98" r:id="rId67" xr:uid="{C2F979F8-CA76-4D4D-950C-5DA192A1704D}"/>
+    <hyperlink ref="A99" r:id="rId68" xr:uid="{235AA574-21B4-4120-9E2A-AF92C8F63BCF}"/>
+    <hyperlink ref="A100" r:id="rId69" xr:uid="{233D8829-0413-42FB-975B-744E92254D18}"/>
+    <hyperlink ref="A101" r:id="rId70" xr:uid="{66DA3037-2148-4B17-8574-FA464DD800A9}"/>
+    <hyperlink ref="A102" r:id="rId71" xr:uid="{1E7C08B5-CD5F-4FF0-89E5-14BE611B4EAD}"/>
+    <hyperlink ref="A103" r:id="rId72" xr:uid="{454453A0-B2E9-42B9-BDB5-4944EA4D6E1D}"/>
+    <hyperlink ref="A104" r:id="rId73" xr:uid="{2E9C7AB9-DE8A-4A68-B988-412D79010433}"/>
+    <hyperlink ref="A105" r:id="rId74" xr:uid="{BE97AB44-7D49-4578-9030-4E8B84DC0F76}"/>
+    <hyperlink ref="A106" r:id="rId75" xr:uid="{7230BA75-4A10-4261-84EC-01BC329910EC}"/>
+    <hyperlink ref="A107" r:id="rId76" xr:uid="{9A2B5275-DFBF-4694-B53A-D925ECF02FC6}"/>
+    <hyperlink ref="A108" r:id="rId77" xr:uid="{34895738-17B5-4525-B963-84A567D843B8}"/>
+    <hyperlink ref="A109" r:id="rId78" xr:uid="{D5EEBC72-BA27-4B74-92DB-D8821558C974}"/>
+    <hyperlink ref="A110" r:id="rId79" xr:uid="{1D4BF4B2-122B-468E-B262-66B134762E6A}"/>
+    <hyperlink ref="A111" r:id="rId80" xr:uid="{3BC65187-8D95-4F69-AA74-723C5F11003D}"/>
+    <hyperlink ref="A112" r:id="rId81" xr:uid="{BB19F90C-0FAB-4C4F-B0CA-9FBCFDC4875E}"/>
+    <hyperlink ref="A113" r:id="rId82" xr:uid="{F0195457-B682-4C57-ACB9-67DCEB279CAB}"/>
+    <hyperlink ref="A114" r:id="rId83" xr:uid="{06D9CE8F-A9A0-4B81-B44B-61A04398FF66}"/>
+    <hyperlink ref="A115" r:id="rId84" xr:uid="{CAFC43B8-F6D2-4D48-8AFD-9EB9AEA55945}"/>
+    <hyperlink ref="A117" r:id="rId85" xr:uid="{0E35D408-1A04-4F49-A32D-3A6B79B14BFD}"/>
+    <hyperlink ref="A118" r:id="rId86" xr:uid="{80B3A772-04C2-488F-A0DA-DB80BEDA0590}"/>
+    <hyperlink ref="A119" r:id="rId87" xr:uid="{C115EA34-EE3B-4DEE-A4A0-82D1362EB2BE}"/>
+    <hyperlink ref="A120" r:id="rId88" xr:uid="{BAB4A183-1468-458D-B5B1-2C138E49CFDB}"/>
+    <hyperlink ref="A121" r:id="rId89" xr:uid="{781BE4D3-4232-476F-9DBB-A0BFBC820075}"/>
+    <hyperlink ref="A122" r:id="rId90" xr:uid="{62DC21A5-2BF2-4669-B94B-ABA434E69C5C}"/>
+    <hyperlink ref="A123" r:id="rId91" xr:uid="{DB9C7DD4-5A56-44BF-9455-CF1300C2CABF}"/>
+    <hyperlink ref="A124" r:id="rId92" xr:uid="{3F17BB3C-0054-472D-A0EB-E5191241E79D}"/>
+    <hyperlink ref="B124" r:id="rId93" xr:uid="{51462D44-4E19-41F7-A512-9FC32CF52581}"/>
+    <hyperlink ref="A125" r:id="rId94" xr:uid="{823A2906-269C-4D34-84BC-CFAA3837EACB}"/>
+    <hyperlink ref="A126" r:id="rId95" xr:uid="{FBC05216-AD1B-41AA-B897-49F4270B031B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId96"/>
 </worksheet>
 </file>
</xml_diff>